<commit_message>
compara en casa terminado
</commit_message>
<xml_diff>
--- a/scrap_1/data_perfiles.xlsx
+++ b/scrap_1/data_perfiles.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\proyectos\scrap_1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35287EEB-595C-495C-96FA-73EE531F4AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -82,14 +76,17 @@
     <t>04/06/2021</t>
   </si>
   <si>
+    <t>11/06/2021</t>
+  </si>
+  <si>
     <t>nan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,19 +149,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -206,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,27 +227,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,24 +261,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -483,20 +436,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +487,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>2</v>
       </c>
@@ -551,25 +498,25 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2">
         <v>1493.11</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2">
         <v>2182</v>
@@ -584,7 +531,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>2</v>
       </c>
@@ -595,25 +542,25 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3">
-        <v>4560.6499999999996</v>
+        <v>4560.65</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3">
         <v>8829.5</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I3">
         <v>5725.2</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K3">
         <v>2585</v>
@@ -628,7 +575,7 @@
         <v>4449.2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>2</v>
       </c>
@@ -642,22 +589,22 @@
         <v>5006.92</v>
       </c>
       <c r="E4">
-        <v>4880.6499999999996</v>
+        <v>4880.65</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G4">
         <v>7791.74</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I4">
         <v>5178.43</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K4">
         <v>7421</v>
@@ -666,13 +613,13 @@
         <v>6817.37</v>
       </c>
       <c r="M4">
-        <v>4909.9799999999996</v>
+        <v>4909.98</v>
       </c>
       <c r="N4">
         <v>5131.7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>2</v>
       </c>
@@ -716,7 +663,7 @@
         <v>6308.4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>2</v>
       </c>
@@ -739,7 +686,7 @@
         <v>9535.76</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I6">
         <v>9711.33</v>
@@ -751,16 +698,16 @@
         <v>16107</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N6">
-        <v>10219.299999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10219.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>3</v>
       </c>
@@ -771,40 +718,40 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>3</v>
       </c>
@@ -815,40 +762,40 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>4814.43</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8">
         <v>10853.51</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>3</v>
       </c>
@@ -865,34 +812,34 @@
         <v>5748.03</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9">
         <v>9503.17</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10">
         <v>3</v>
       </c>
@@ -918,25 +865,25 @@
         <v>9029.27</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J10">
         <v>13546</v>
       </c>
       <c r="K10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11">
         <v>3</v>
       </c>
@@ -953,34 +900,34 @@
         <v>10273.25</v>
       </c>
       <c r="F11">
-        <v>18983.939999999999</v>
+        <v>18983.94</v>
       </c>
       <c r="G11">
-        <v>9823.61</v>
+        <v>9823.610000000001</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J11">
         <v>21250</v>
       </c>
       <c r="K11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12">
         <v>4</v>
       </c>
@@ -991,31 +938,31 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I12">
         <v>1750.05</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K12">
         <v>3092</v>
       </c>
       <c r="L12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M12">
         <v>831.58</v>
@@ -1024,7 +971,7 @@
         <v>2522</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1035,31 +982,31 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G13">
         <v>15275.5</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I13">
         <v>11734.34</v>
       </c>
       <c r="J13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K13">
         <v>4044</v>
       </c>
       <c r="L13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M13">
         <v>12914.09</v>
@@ -1068,7 +1015,7 @@
         <v>4696.3</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1082,28 +1029,28 @@
         <v>7884.45</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G14">
         <v>13304.05</v>
       </c>
       <c r="H14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I14">
-        <v>9957.2000000000007</v>
+        <v>9957.200000000001</v>
       </c>
       <c r="J14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K14">
         <v>15151</v>
       </c>
       <c r="L14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M14">
         <v>11863.51</v>
@@ -1112,7 +1059,7 @@
         <v>5397.7</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1126,7 +1073,7 @@
         <v>7820.75</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F15">
         <v>15479.36</v>
@@ -1147,7 +1094,7 @@
         <v>15673</v>
       </c>
       <c r="L15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M15">
         <v>14503.51</v>
@@ -1156,7 +1103,7 @@
         <v>6885.9</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1167,10 +1114,10 @@
         <v>19</v>
       </c>
       <c r="D16">
-        <v>9894.31</v>
+        <v>9894.309999999999</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F16">
         <v>23887.58</v>
@@ -1179,7 +1126,7 @@
         <v>13718.34</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I16">
         <v>21443.98</v>
@@ -1191,16 +1138,16 @@
         <v>27589</v>
       </c>
       <c r="L16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N16">
         <v>14833.7</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1211,28 +1158,28 @@
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I17">
         <v>1493.11</v>
       </c>
       <c r="J17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L17">
         <v>1835.29</v>
@@ -1244,7 +1191,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1255,28 +1202,28 @@
         <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E18">
         <v>3178.74</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G18">
         <v>4047.89</v>
       </c>
       <c r="H18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I18">
         <v>3358.42</v>
       </c>
       <c r="J18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L18">
         <v>3812.41</v>
@@ -1288,7 +1235,7 @@
         <v>2537.5</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1305,22 +1252,22 @@
         <v>3424.51</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G19">
         <v>4466.03</v>
       </c>
       <c r="H19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I19">
         <v>2939.3</v>
       </c>
       <c r="J19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L19">
         <v>4123.2</v>
@@ -1332,7 +1279,7 @@
         <v>2925.3</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1352,22 +1299,22 @@
         <v>5609.5</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H20">
         <v>3295.76</v>
       </c>
       <c r="I20">
-        <v>4665.5600000000004</v>
+        <v>4665.56</v>
       </c>
       <c r="J20">
         <v>5258</v>
       </c>
       <c r="K20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L20">
-        <v>4339.1899999999996</v>
+        <v>4339.19</v>
       </c>
       <c r="M20">
         <v>3413.15</v>
@@ -1376,7 +1323,7 @@
         <v>3510.5</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1399,25 +1346,1125 @@
         <v>6250.28</v>
       </c>
       <c r="H21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M21">
         <v>6570.87</v>
       </c>
       <c r="N21">
         <v>5821.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22">
+        <v>1493.11</v>
+      </c>
+      <c r="J22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22">
+        <v>2182</v>
+      </c>
+      <c r="L22">
+        <v>1835.29</v>
+      </c>
+      <c r="M22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N22">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23">
+        <v>3214.92</v>
+      </c>
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23">
+        <v>4047.89</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23">
+        <v>3358.42</v>
+      </c>
+      <c r="J23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23">
+        <v>2602</v>
+      </c>
+      <c r="L23">
+        <v>3812.41</v>
+      </c>
+      <c r="M23" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23">
+        <v>2537.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>3364.04</v>
+      </c>
+      <c r="E24">
+        <v>3468.06</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24">
+        <v>4466.03</v>
+      </c>
+      <c r="H24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24">
+        <v>2939.3</v>
+      </c>
+      <c r="J24" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24">
+        <v>4705</v>
+      </c>
+      <c r="L24">
+        <v>4123.2</v>
+      </c>
+      <c r="M24" t="s">
+        <v>21</v>
+      </c>
+      <c r="N24">
+        <v>2925.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>3262.85</v>
+      </c>
+      <c r="E25">
+        <v>3500.68</v>
+      </c>
+      <c r="F25">
+        <v>5735.38</v>
+      </c>
+      <c r="G25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25">
+        <v>3295.76</v>
+      </c>
+      <c r="I25">
+        <v>4665.56</v>
+      </c>
+      <c r="J25">
+        <v>5258</v>
+      </c>
+      <c r="K25">
+        <v>4839</v>
+      </c>
+      <c r="L25">
+        <v>4339.19</v>
+      </c>
+      <c r="M25" t="s">
+        <v>21</v>
+      </c>
+      <c r="N25">
+        <v>3510.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>4492.57</v>
+      </c>
+      <c r="E26">
+        <v>5840.52</v>
+      </c>
+      <c r="F26">
+        <v>8236.33</v>
+      </c>
+      <c r="G26">
+        <v>6250.28</v>
+      </c>
+      <c r="H26" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" t="s">
+        <v>21</v>
+      </c>
+      <c r="M26" t="s">
+        <v>21</v>
+      </c>
+      <c r="N26">
+        <v>5821.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27">
+        <v>1493.11</v>
+      </c>
+      <c r="J27" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27">
+        <v>2182</v>
+      </c>
+      <c r="L27">
+        <v>1835.29</v>
+      </c>
+      <c r="M27" t="s">
+        <v>21</v>
+      </c>
+      <c r="N27">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28">
+        <v>4627.45</v>
+      </c>
+      <c r="F28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28">
+        <v>8829.5</v>
+      </c>
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28">
+        <v>5725.2</v>
+      </c>
+      <c r="J28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28">
+        <v>2585</v>
+      </c>
+      <c r="L28">
+        <v>6506.57</v>
+      </c>
+      <c r="M28" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28">
+        <v>4449.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29">
+        <v>5006.92</v>
+      </c>
+      <c r="E29">
+        <v>4956.55</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29">
+        <v>7791.74</v>
+      </c>
+      <c r="H29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29">
+        <v>5178.43</v>
+      </c>
+      <c r="J29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29">
+        <v>7421</v>
+      </c>
+      <c r="L29">
+        <v>6817.37</v>
+      </c>
+      <c r="M29" t="s">
+        <v>21</v>
+      </c>
+      <c r="N29">
+        <v>5131.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <v>4956.47</v>
+      </c>
+      <c r="E30">
+        <v>5054.78</v>
+      </c>
+      <c r="F30">
+        <v>13903.95</v>
+      </c>
+      <c r="G30">
+        <v>6379</v>
+      </c>
+      <c r="H30">
+        <v>6187.25</v>
+      </c>
+      <c r="I30">
+        <v>6575.8</v>
+      </c>
+      <c r="J30">
+        <v>8808</v>
+      </c>
+      <c r="K30">
+        <v>7729</v>
+      </c>
+      <c r="L30">
+        <v>7377.97</v>
+      </c>
+      <c r="M30" t="s">
+        <v>21</v>
+      </c>
+      <c r="N30">
+        <v>6308.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31">
+        <v>6013.62</v>
+      </c>
+      <c r="E31">
+        <v>7852.49</v>
+      </c>
+      <c r="F31">
+        <v>20790.88</v>
+      </c>
+      <c r="G31">
+        <v>9535.76</v>
+      </c>
+      <c r="H31" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31">
+        <v>9711.33</v>
+      </c>
+      <c r="J31">
+        <v>16283</v>
+      </c>
+      <c r="K31">
+        <v>16107</v>
+      </c>
+      <c r="L31" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" t="s">
+        <v>21</v>
+      </c>
+      <c r="N31">
+        <v>10219.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" t="s">
+        <v>21</v>
+      </c>
+      <c r="J32" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32">
+        <v>2182</v>
+      </c>
+      <c r="L32">
+        <v>1835.29</v>
+      </c>
+      <c r="M32" t="s">
+        <v>21</v>
+      </c>
+      <c r="N32">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33">
+        <v>5052.03</v>
+      </c>
+      <c r="F33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33">
+        <v>10853.51</v>
+      </c>
+      <c r="H33" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33">
+        <v>2899</v>
+      </c>
+      <c r="L33">
+        <v>9094.66</v>
+      </c>
+      <c r="M33" t="s">
+        <v>21</v>
+      </c>
+      <c r="N33">
+        <v>6136.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34">
+        <v>6075.34</v>
+      </c>
+      <c r="E34">
+        <v>6057.29</v>
+      </c>
+      <c r="F34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34">
+        <v>9503.17</v>
+      </c>
+      <c r="H34" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34">
+        <v>9543</v>
+      </c>
+      <c r="L34">
+        <v>9405.48</v>
+      </c>
+      <c r="M34" t="s">
+        <v>21</v>
+      </c>
+      <c r="N34">
+        <v>7079.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35">
+        <v>6081.51</v>
+      </c>
+      <c r="E35">
+        <v>6174.59</v>
+      </c>
+      <c r="F35">
+        <v>12927.04</v>
+      </c>
+      <c r="G35">
+        <v>7676.84</v>
+      </c>
+      <c r="H35">
+        <v>9029.27</v>
+      </c>
+      <c r="I35" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35">
+        <v>13546</v>
+      </c>
+      <c r="K35">
+        <v>9967</v>
+      </c>
+      <c r="L35">
+        <v>10297.09</v>
+      </c>
+      <c r="M35" t="s">
+        <v>21</v>
+      </c>
+      <c r="N35">
+        <v>8855</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>7644.54</v>
+      </c>
+      <c r="E36">
+        <v>10917</v>
+      </c>
+      <c r="F36">
+        <v>19201.82</v>
+      </c>
+      <c r="G36">
+        <v>9823.610000000001</v>
+      </c>
+      <c r="H36" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36">
+        <v>21250</v>
+      </c>
+      <c r="K36">
+        <v>19573</v>
+      </c>
+      <c r="L36" t="s">
+        <v>21</v>
+      </c>
+      <c r="M36" t="s">
+        <v>21</v>
+      </c>
+      <c r="N36">
+        <v>14753.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37">
+        <v>1750.05</v>
+      </c>
+      <c r="J37" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37">
+        <v>3092</v>
+      </c>
+      <c r="L37" t="s">
+        <v>21</v>
+      </c>
+      <c r="M37" t="s">
+        <v>21</v>
+      </c>
+      <c r="N37">
+        <v>2522</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38">
+        <v>8256.5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38">
+        <v>15275.5</v>
+      </c>
+      <c r="H38" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38">
+        <v>11734.34</v>
+      </c>
+      <c r="J38" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38">
+        <v>4044</v>
+      </c>
+      <c r="L38" t="s">
+        <v>21</v>
+      </c>
+      <c r="M38" t="s">
+        <v>21</v>
+      </c>
+      <c r="N38">
+        <v>4696.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39">
+        <v>7884.45</v>
+      </c>
+      <c r="E39">
+        <v>8814.309999999999</v>
+      </c>
+      <c r="F39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39">
+        <v>13304.05</v>
+      </c>
+      <c r="H39" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39">
+        <v>9957.200000000001</v>
+      </c>
+      <c r="J39" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39">
+        <v>15151</v>
+      </c>
+      <c r="L39" t="s">
+        <v>21</v>
+      </c>
+      <c r="M39" t="s">
+        <v>21</v>
+      </c>
+      <c r="N39">
+        <v>5397.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40">
+        <v>7820.75</v>
+      </c>
+      <c r="E40">
+        <v>8972.610000000001</v>
+      </c>
+      <c r="F40">
+        <v>16361.99</v>
+      </c>
+      <c r="G40">
+        <v>10647.45</v>
+      </c>
+      <c r="H40">
+        <v>10795.86</v>
+      </c>
+      <c r="I40">
+        <v>12644.05</v>
+      </c>
+      <c r="J40">
+        <v>22509</v>
+      </c>
+      <c r="K40">
+        <v>15673</v>
+      </c>
+      <c r="L40" t="s">
+        <v>21</v>
+      </c>
+      <c r="M40" t="s">
+        <v>21</v>
+      </c>
+      <c r="N40">
+        <v>6885.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41">
+        <v>9894.309999999999</v>
+      </c>
+      <c r="E41">
+        <v>12164.11</v>
+      </c>
+      <c r="F41">
+        <v>25294.6</v>
+      </c>
+      <c r="G41">
+        <v>13718.34</v>
+      </c>
+      <c r="H41" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41">
+        <v>21443.98</v>
+      </c>
+      <c r="J41">
+        <v>26187</v>
+      </c>
+      <c r="K41">
+        <v>27589</v>
+      </c>
+      <c r="L41" t="s">
+        <v>21</v>
+      </c>
+      <c r="M41" t="s">
+        <v>21</v>
+      </c>
+      <c r="N41">
+        <v>14833.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42">
+        <v>1493.11</v>
+      </c>
+      <c r="J42" t="s">
+        <v>21</v>
+      </c>
+      <c r="K42">
+        <v>2182</v>
+      </c>
+      <c r="L42">
+        <v>1835.29</v>
+      </c>
+      <c r="M42" t="s">
+        <v>21</v>
+      </c>
+      <c r="N42">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43">
+        <v>3056.1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43">
+        <v>6434.62</v>
+      </c>
+      <c r="H43" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43">
+        <v>4325.8</v>
+      </c>
+      <c r="J43" t="s">
+        <v>21</v>
+      </c>
+      <c r="K43">
+        <v>2436</v>
+      </c>
+      <c r="L43">
+        <v>5205.31</v>
+      </c>
+      <c r="M43" t="s">
+        <v>21</v>
+      </c>
+      <c r="N43">
+        <v>3768.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44">
+        <v>4068.71</v>
+      </c>
+      <c r="E44">
+        <v>3285.38</v>
+      </c>
+      <c r="F44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44">
+        <v>5766.75</v>
+      </c>
+      <c r="H44" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44">
+        <v>3854.91</v>
+      </c>
+      <c r="J44" t="s">
+        <v>21</v>
+      </c>
+      <c r="K44">
+        <v>5711</v>
+      </c>
+      <c r="L44">
+        <v>5516.1</v>
+      </c>
+      <c r="M44" t="s">
+        <v>21</v>
+      </c>
+      <c r="N44">
+        <v>4345.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45">
+        <v>3998.77</v>
+      </c>
+      <c r="E45">
+        <v>3344.34</v>
+      </c>
+      <c r="F45">
+        <v>7766.49</v>
+      </c>
+      <c r="G45">
+        <v>4843.35</v>
+      </c>
+      <c r="H45">
+        <v>4474.06</v>
+      </c>
+      <c r="I45">
+        <v>4895.13</v>
+      </c>
+      <c r="J45">
+        <v>7351</v>
+      </c>
+      <c r="K45">
+        <v>5920</v>
+      </c>
+      <c r="L45">
+        <v>5910.24</v>
+      </c>
+      <c r="M45" t="s">
+        <v>21</v>
+      </c>
+      <c r="N45">
+        <v>5292.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46">
+        <v>4949.94</v>
+      </c>
+      <c r="E46">
+        <v>6601.92</v>
+      </c>
+      <c r="F46">
+        <v>11464.04</v>
+      </c>
+      <c r="G46">
+        <v>7851.08</v>
+      </c>
+      <c r="H46" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46">
+        <v>11612</v>
+      </c>
+      <c r="K46">
+        <v>11936</v>
+      </c>
+      <c r="L46" t="s">
+        <v>21</v>
+      </c>
+      <c r="M46" t="s">
+        <v>21</v>
+      </c>
+      <c r="N46">
+        <v>8354.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>